<commit_message>
changed filling zhr_izol.xslx for new order (22/03/2022)
</commit_message>
<xml_diff>
--- a/Excell/zhr_izol.xlsx
+++ b/Excell/zhr_izol.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF666670-9FEE-434E-A0E6-D1110CB04AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tittle" sheetId="1" r:id="rId1"/>
@@ -235,7 +236,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -670,8 +671,59 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -688,57 +740,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -748,6 +749,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -796,7 +800,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -829,9 +833,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -864,6 +885,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1039,7 +1077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:BY145"/>
   <sheetViews>
@@ -1054,85 +1092,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
-      <c r="AW1" s="51"/>
-      <c r="AX1" s="51"/>
-      <c r="AY1" s="51"/>
-      <c r="AZ1" s="51"/>
-      <c r="BA1" s="51"/>
-      <c r="BB1" s="51"/>
-      <c r="BC1" s="51"/>
-      <c r="BD1" s="51"/>
-      <c r="BE1" s="51"/>
-      <c r="BF1" s="51"/>
-      <c r="BG1" s="51"/>
-      <c r="BH1" s="51"/>
-      <c r="BI1" s="51"/>
-      <c r="BJ1" s="51"/>
-      <c r="BK1" s="51"/>
-      <c r="BL1" s="51"/>
-      <c r="BM1" s="51"/>
-      <c r="BN1" s="51"/>
-      <c r="BO1" s="51"/>
-      <c r="BP1" s="51"/>
-      <c r="BQ1" s="51"/>
-      <c r="BR1" s="51"/>
-      <c r="BS1" s="51"/>
-      <c r="BT1" s="51"/>
-      <c r="BU1" s="51"/>
-      <c r="BV1" s="51"/>
-      <c r="BW1" s="51"/>
-      <c r="BX1" s="51"/>
-      <c r="BY1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="52"/>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
+      <c r="AK1" s="52"/>
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="52"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AQ1" s="52"/>
+      <c r="AR1" s="52"/>
+      <c r="AS1" s="52"/>
+      <c r="AT1" s="52"/>
+      <c r="AU1" s="52"/>
+      <c r="AV1" s="52"/>
+      <c r="AW1" s="52"/>
+      <c r="AX1" s="52"/>
+      <c r="AY1" s="52"/>
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="52"/>
+      <c r="BF1" s="52"/>
+      <c r="BG1" s="52"/>
+      <c r="BH1" s="52"/>
+      <c r="BI1" s="52"/>
+      <c r="BJ1" s="52"/>
+      <c r="BK1" s="52"/>
+      <c r="BL1" s="52"/>
+      <c r="BM1" s="52"/>
+      <c r="BN1" s="52"/>
+      <c r="BO1" s="52"/>
+      <c r="BP1" s="52"/>
+      <c r="BQ1" s="52"/>
+      <c r="BR1" s="52"/>
+      <c r="BS1" s="52"/>
+      <c r="BT1" s="52"/>
+      <c r="BU1" s="52"/>
+      <c r="BV1" s="52"/>
+      <c r="BW1" s="52"/>
+      <c r="BX1" s="52"/>
+      <c r="BY1" s="52"/>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.3">
       <c r="AN2" s="9" t="s">
@@ -1140,85 +1178,85 @@
       </c>
     </row>
     <row r="3" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="51"/>
-      <c r="AE3" s="51"/>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="51"/>
-      <c r="AN3" s="51"/>
-      <c r="AO3" s="51"/>
-      <c r="AP3" s="51"/>
-      <c r="AQ3" s="51"/>
-      <c r="AR3" s="51"/>
-      <c r="AS3" s="51"/>
-      <c r="AT3" s="51"/>
-      <c r="AU3" s="51"/>
-      <c r="AV3" s="51"/>
-      <c r="AW3" s="51"/>
-      <c r="AX3" s="51"/>
-      <c r="AY3" s="51"/>
-      <c r="AZ3" s="51"/>
-      <c r="BA3" s="51"/>
-      <c r="BB3" s="51"/>
-      <c r="BC3" s="51"/>
-      <c r="BD3" s="51"/>
-      <c r="BE3" s="51"/>
-      <c r="BF3" s="51"/>
-      <c r="BG3" s="51"/>
-      <c r="BH3" s="51"/>
-      <c r="BI3" s="51"/>
-      <c r="BJ3" s="51"/>
-      <c r="BK3" s="51"/>
-      <c r="BL3" s="51"/>
-      <c r="BM3" s="51"/>
-      <c r="BN3" s="51"/>
-      <c r="BO3" s="51"/>
-      <c r="BP3" s="51"/>
-      <c r="BQ3" s="51"/>
-      <c r="BR3" s="51"/>
-      <c r="BS3" s="51"/>
-      <c r="BT3" s="51"/>
-      <c r="BU3" s="51"/>
-      <c r="BV3" s="51"/>
-      <c r="BW3" s="51"/>
-      <c r="BX3" s="51"/>
-      <c r="BY3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="52"/>
+      <c r="AB3" s="52"/>
+      <c r="AC3" s="52"/>
+      <c r="AD3" s="52"/>
+      <c r="AE3" s="52"/>
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="52"/>
+      <c r="AH3" s="52"/>
+      <c r="AI3" s="52"/>
+      <c r="AJ3" s="52"/>
+      <c r="AK3" s="52"/>
+      <c r="AL3" s="52"/>
+      <c r="AM3" s="52"/>
+      <c r="AN3" s="52"/>
+      <c r="AO3" s="52"/>
+      <c r="AP3" s="52"/>
+      <c r="AQ3" s="52"/>
+      <c r="AR3" s="52"/>
+      <c r="AS3" s="52"/>
+      <c r="AT3" s="52"/>
+      <c r="AU3" s="52"/>
+      <c r="AV3" s="52"/>
+      <c r="AW3" s="52"/>
+      <c r="AX3" s="52"/>
+      <c r="AY3" s="52"/>
+      <c r="AZ3" s="52"/>
+      <c r="BA3" s="52"/>
+      <c r="BB3" s="52"/>
+      <c r="BC3" s="52"/>
+      <c r="BD3" s="52"/>
+      <c r="BE3" s="52"/>
+      <c r="BF3" s="52"/>
+      <c r="BG3" s="52"/>
+      <c r="BH3" s="52"/>
+      <c r="BI3" s="52"/>
+      <c r="BJ3" s="52"/>
+      <c r="BK3" s="52"/>
+      <c r="BL3" s="52"/>
+      <c r="BM3" s="52"/>
+      <c r="BN3" s="52"/>
+      <c r="BO3" s="52"/>
+      <c r="BP3" s="52"/>
+      <c r="BQ3" s="52"/>
+      <c r="BR3" s="52"/>
+      <c r="BS3" s="52"/>
+      <c r="BT3" s="52"/>
+      <c r="BU3" s="52"/>
+      <c r="BV3" s="52"/>
+      <c r="BW3" s="52"/>
+      <c r="BX3" s="52"/>
+      <c r="BY3" s="52"/>
     </row>
     <row r="4" spans="1:77" x14ac:dyDescent="0.3">
       <c r="D4" s="11"/>
@@ -7111,10 +7149,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="145" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="145" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -7136,8 +7174,8 @@
     <col min="14" max="14" width="9.7109375" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" customWidth="1"/>
     <col min="16" max="16" width="5.5703125" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
     <col min="19" max="19" width="7.5703125" customWidth="1"/>
     <col min="20" max="20" width="11.140625" customWidth="1"/>
     <col min="21" max="21" width="18.140625" customWidth="1"/>
@@ -7147,142 +7185,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="59" t="s">
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="64" t="s">
+      <c r="K1" s="61"/>
+      <c r="L1" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="63" t="s">
+      <c r="N1" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="54" t="s">
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="55" t="s">
+      <c r="U1" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="52" t="s">
+      <c r="V1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
     </row>
     <row r="2" spans="1:24" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="60" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="69"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59" t="s">
+      <c r="H2" s="56"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="58" t="s">
+      <c r="L2" s="60"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="57" t="s">
+      <c r="O2" s="66"/>
+      <c r="P2" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="53" t="s">
+      <c r="Q2" s="71"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="53" t="s">
+      <c r="W2" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="70" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="66"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="54"/>
       <c r="G3" s="41" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="62"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="65"/>
       <c r="N3" s="44" t="s">
         <v>43</v>
       </c>
       <c r="O3" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="70"/>
+      <c r="W3" s="70"/>
+      <c r="X3" s="70"/>
     </row>
     <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42">
@@ -8455,23 +8493,6 @@
     <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="L1:L3"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="M1:M3"/>
-    <mergeCell ref="N1:P1"/>
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
@@ -8481,6 +8502,23 @@
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -8491,10 +8529,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8503,7 +8541,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="51" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>